<commit_message>
WR update.  Method update
WR update.  Method update.
</commit_message>
<xml_diff>
--- a/Arizona/WaterAllocation/AZ_GW_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Arizona/WaterAllocation/AZ_GW_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Arizona\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301D5D53-4C2A-4105-A06C-A30BF94A2CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39E3CF-4879-4C1C-8B51-02922370EC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12456" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="309">
   <si>
     <t>Name</t>
   </si>
@@ -798,16 +798,7 @@
     <t>(blank)</t>
   </si>
   <si>
-    <t>Water Rights</t>
-  </si>
-  <si>
-    <t>Arizona Water Rights</t>
-  </si>
-  <si>
     <t>http://gisdata-azwater.opendata.arcgis.com/</t>
-  </si>
-  <si>
-    <t>Adjudicated</t>
   </si>
   <si>
     <t>ADWR_Allocation All</t>
@@ -962,6 +953,23 @@
   </si>
   <si>
     <t>AZwr_WR + counter</t>
+  </si>
+  <si>
+    <t>Arizona Water Rights Method</t>
+  </si>
+  <si>
+    <t>https://new.azwater.gov/surface-water</t>
+  </si>
+  <si>
+    <t>Legal Processes</t>
+  </si>
+  <si>
+    <t>The data on this website was developed by the Arizona Department of Water Resources (“Department”), for uses beneficial to the State of Arizona. The information is available to interested members of the public. While the Department believes the information to be reliable and made efforts to assure its reliability at the time the information was compiled, the information is provided “as is.” The Department is not responsible for the accuracy, completeness, quality or legal sufficiency of the information. Any expressed or implied warranties, including, but not limited to, the implied warranties of merchantability and fitness for the purpose ARE SPECIFICALLY DISCLAIMED. Neither the Department nor the State of Arizona shall be held liable for any direct, indirect, incidental, special, exemplary or consequential damages (including, but not limited to: procurement of substitute goods or services; loss of use, data or profits; or business interruption), however caused and on any theory of liability, whether in contract, strict liability or its aggregate use with other information, data or programs. The information contained in each of the basin descriptions at this site was obtained from information on file in the offices of the Department of Water Resources and limited additional information. Recent studies may contain additional, more up-to-date information. The State of Arizona and the Department of Water Resources hereby specifically retain any intellectual property interest, including copyright, that it may hold in the information provided, whether the information is in the form of data, files, text images, photography or maps.
+The Department requests that persons receiving and using this information not make it available to others for their re-use. Instead, interested third parties should be encouraged to request copies directly from the Department, the source that developed the information, in order to provide the greatest degree of reliability.
+The Groundwater Site Inventory (GWSI) is ADWR's main repository for state-wide groundwater data. The GWSI consists of field-verified data regarding wells and springs collected by personnel from ADWR's Hydrology Division's Field Services Section, the U.S. Geological Survey, and other co-operating agencies. The information in GWSI is constantly being updated by ongoing field investigations and through a state-wide network of water level and water quality monitoring sites.</t>
+  </si>
+  <si>
+    <t>"https://www.azwater.gov/gwsi/Detail.aspx?SiteID=" + df_GWSI_WR['SITE_ID'].astype(str)</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1715,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1763,19 +1771,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -1863,9 +1865,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1908,7 +1907,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1924,9 +1923,6 @@
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1938,9 +1934,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1986,9 +1979,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2353,12 +2343,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="64" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="64" t="s">
         <v>228</v>
       </c>
       <c r="B1" t="s">
@@ -2366,7 +2356,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="64" t="s">
         <v>229</v>
       </c>
       <c r="B2" t="s">
@@ -2374,21 +2364,21 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="B6" s="59" t="s">
-        <v>287</v>
+      <c r="B6" s="56" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="59"/>
+      <c r="B7" s="56"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" s="59"/>
+      <c r="B8" s="56"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="64" t="s">
         <v>231</v>
       </c>
       <c r="B13" t="s">
@@ -2402,28 +2392,28 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="77"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="90" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="90" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
-        <v>300</v>
-      </c>
-      <c r="B20" s="95" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="95" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2438,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2606DDD-D901-4365-BB8D-3E6142C84460}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,7 +2438,7 @@
     <col min="2" max="2" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.5546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.109375" style="5" bestFit="1" customWidth="1"/>
@@ -2509,13 +2499,13 @@
       <c r="D3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="32" t="s">
+      <c r="E3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -2524,7 +2514,7 @@
       <c r="I3" s="17">
         <v>11</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2532,27 +2522,27 @@
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>302</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="C4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2570,17 +2560,17 @@
         <v>20</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+        <v>276</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="57" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2597,18 +2587,18 @@
       <c r="D6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="63">
         <v>0.5</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="57" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2625,18 +2615,18 @@
       <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="60" t="s">
+      <c r="I7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="57" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2653,22 +2643,22 @@
       <c r="D8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="348" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -2682,15 +2672,15 @@
         <v>38</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+        <v>307</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="18"/>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="57" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2708,21 +2698,21 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+        <v>304</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="57" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -2735,18 +2725,18 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="81" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="76" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="57" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2763,18 +2753,18 @@
       <c r="D12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="E12" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="57" t="s">
         <v>208</v>
       </c>
     </row>
@@ -2783,7 +2773,7 @@
     <sortCondition ref="A18:A26"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{D66E14E7-A1AF-4AB3-BFD3-1B9BE5502863}"/>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{285986D7-FBD1-4819-BEDF-90CEE516A973}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2865,16 +2855,16 @@
       <c r="D3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I3" s="17">
         <v>16</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2882,27 +2872,27 @@
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>303</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="C4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2922,15 +2912,15 @@
       <c r="E5" s="17">
         <v>1</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="17">
         <v>1</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="57" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2950,15 +2940,15 @@
       <c r="E6" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="57" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2978,15 +2968,15 @@
       <c r="E7" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="57" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3006,15 +2996,15 @@
       <c r="E8" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3034,15 +3024,15 @@
       <c r="E9" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="57" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3062,15 +3052,15 @@
       <c r="E10" s="17">
         <v>10</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="17">
         <v>10</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="57" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3088,17 +3078,17 @@
         <v>20</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+        <v>254</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="57" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3118,15 +3108,15 @@
       <c r="E12" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="57" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3146,15 +3136,15 @@
       <c r="E13" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J13" s="60" t="s">
+      <c r="J13" s="57" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3242,13 +3232,13 @@
       <c r="D3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="29" t="s">
+      <c r="E3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -3257,7 +3247,7 @@
       <c r="I3" s="18">
         <v>1</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3265,27 +3255,27 @@
       <c r="A4" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="C4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3302,18 +3292,18 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="81" t="s">
-        <v>278</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="E5" s="76" t="s">
+        <v>275</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="57" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3331,17 +3321,17 @@
         <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+        <v>274</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="57" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3358,18 +3348,18 @@
       <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="81" t="s">
-        <v>259</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="E7" s="76" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="57" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3387,17 +3377,17 @@
         <v>38</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+        <v>257</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3415,17 +3405,17 @@
         <v>38</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+        <v>258</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="57" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3443,17 +3433,17 @@
         <v>38</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+        <v>259</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="57" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3470,18 +3460,18 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="81" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="76" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="57" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3499,17 +3489,17 @@
         <v>38</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+        <v>260</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="57" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3626,20 +3616,20 @@
       <c r="D3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="19"/>
+      <c r="E3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="17">
         <v>34658</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3647,25 +3637,25 @@
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>265</v>
-      </c>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="19"/>
+      <c r="C4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3682,16 +3672,16 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="60" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="57" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3708,16 +3698,16 @@
       <c r="D6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="60" t="s">
+      <c r="F6" s="65"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="57" t="s">
         <v>214</v>
       </c>
     </row>
@@ -3734,16 +3724,16 @@
       <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="19"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="57" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3760,16 +3750,16 @@
       <c r="D8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="68" t="s">
-        <v>264</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="23"/>
+      <c r="E8" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3786,16 +3776,16 @@
       <c r="D9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="68" t="s">
-        <v>294</v>
-      </c>
-      <c r="F9" s="68"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="19"/>
+      <c r="E9" s="65" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="65"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="17">
         <v>17839</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="57" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3812,20 +3802,20 @@
       <c r="D10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="68" t="s">
-        <v>293</v>
-      </c>
-      <c r="F10" s="79" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="23"/>
+      <c r="E10" s="65" t="s">
+        <v>290</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="21"/>
       <c r="I10" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="57" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3921,20 +3911,20 @@
       <c r="D3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="19"/>
+      <c r="E3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="18">
         <v>39035</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3942,27 +3932,27 @@
       <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>267</v>
-      </c>
-      <c r="F4" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="19"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3979,20 +3969,20 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F5" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="19"/>
+      <c r="F5" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="9"/>
       <c r="I5" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="57" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4009,20 +3999,20 @@
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="19"/>
+      <c r="E6" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="9"/>
       <c r="I6" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="57" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4039,50 +4029,50 @@
       <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="61" t="s">
+      <c r="E7" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="58" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="51" t="s">
+      <c r="C8" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="31">
         <v>4236</v>
       </c>
-      <c r="F8" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="23"/>
+      <c r="F8" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="21"/>
       <c r="I8" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4099,18 +4089,18 @@
       <c r="D9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="19"/>
+      <c r="F9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="9"/>
       <c r="I9" s="18"/>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="57" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4127,20 +4117,20 @@
       <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="60" t="s">
+      <c r="F10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="57" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4157,20 +4147,20 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="74" t="s">
+      <c r="E11" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F11" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="61" t="s">
+      <c r="F11" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="58" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4187,78 +4177,78 @@
       <c r="D12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F12" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="61" t="s">
+      <c r="F12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="58" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="G13" s="72" t="s">
-        <v>289</v>
-      </c>
-      <c r="I13" s="62" t="s">
+      <c r="D13" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>286</v>
+      </c>
+      <c r="I13" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="60" t="s">
+      <c r="J13" s="57" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+    <row r="14" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="G14" s="72" t="s">
-        <v>290</v>
-      </c>
-      <c r="I14" s="62">
+      <c r="D14" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G14" s="69" t="s">
+        <v>287</v>
+      </c>
+      <c r="I14" s="59">
         <v>-1067.700435</v>
       </c>
-      <c r="J14" s="60" t="s">
+      <c r="J14" s="57" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4275,20 +4265,20 @@
       <c r="D15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="60" t="s">
+      <c r="F15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="57" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4305,20 +4295,20 @@
       <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="E16" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F16" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="60" t="s">
+      <c r="F16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="57" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4335,17 +4325,17 @@
       <c r="D17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="80" t="s">
+      <c r="E17" s="75" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="45" t="s">
+      <c r="F17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="43" t="s">
         <v>38</v>
       </c>
       <c r="H17"/>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="55" t="s">
         <v>235</v>
       </c>
       <c r="J17"/>
@@ -4361,16 +4351,16 @@
       <c r="D18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="19"/>
+      <c r="E18" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="J18" s="60" t="s">
+      <c r="J18" s="57" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4387,20 +4377,20 @@
       <c r="D19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="G19" s="72" t="s">
-        <v>291</v>
-      </c>
-      <c r="H19" s="23"/>
+      <c r="E19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>288</v>
+      </c>
+      <c r="H19" s="21"/>
       <c r="I19" s="18">
         <v>3703994</v>
       </c>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="57" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4417,20 +4407,20 @@
       <c r="D20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="74" t="s">
+      <c r="E20" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="19"/>
+      <c r="F20" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="9"/>
       <c r="I20" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="J20" s="61" t="s">
+      <c r="J20" s="58" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4447,20 +4437,20 @@
       <c r="D21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="89" t="s">
-        <v>292</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="19"/>
+      <c r="E21" s="84" t="s">
+        <v>289</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="9"/>
       <c r="I21" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="J21" s="60" t="s">
+      <c r="J21" s="57" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4477,24 +4467,24 @@
       <c r="D22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="19"/>
+      <c r="E22" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="9"/>
       <c r="I22" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="J22" s="60" t="s">
+      <c r="J22" s="57" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="69" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>52</v>
       </c>
@@ -4507,20 +4497,20 @@
       <c r="D23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="74" t="s">
+      <c r="E23" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="61" t="s">
+      <c r="F23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="58" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4537,8 +4527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4595,239 +4585,239 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="51" t="s">
+      <c r="C3" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="62">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="59">
         <v>50004</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="52" t="s">
+      <c r="C4" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="62">
+      <c r="E4" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="59">
         <v>43</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="52" t="s">
+      <c r="C5" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="62">
+      <c r="E5" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="59">
         <v>1</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+    <row r="6" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="52" t="s">
+      <c r="C6" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="62">
+      <c r="E6" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="59">
         <v>39035</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="52" t="s">
+      <c r="C7" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="62">
+      <c r="E7" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="59">
         <v>63</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+    <row r="8" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="52" t="s">
+      <c r="C8" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="62">
+      <c r="E8" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="59">
         <v>371091</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
-        <v>305</v>
-      </c>
-      <c r="B9" s="49" t="s">
+    <row r="9" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="96" t="s">
-        <v>306</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="60"/>
-    </row>
-    <row r="10" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="C9" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="57"/>
+    </row>
+    <row r="10" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>280</v>
-      </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="60" t="s">
+      <c r="C10" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="57" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4844,18 +4834,18 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="57" t="s">
-        <v>258</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="60" t="s">
+      <c r="E11" s="54" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="57" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4873,17 +4863,17 @@
         <v>38</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="60" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="57" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4900,18 +4890,18 @@
       <c r="D13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="54" t="s">
-        <v>256</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="60" t="s">
+      <c r="E13" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="57" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4919,355 +4909,355 @@
       <c r="A14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>276</v>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="60" t="s">
+      <c r="C14" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="57" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71" t="s">
+    <row r="15" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="68" t="s">
         <v>238</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F15" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="62">
+      <c r="F15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="59">
         <v>5363</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="57" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71" t="s">
+    <row r="16" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="33" t="s">
+      <c r="D16" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F16" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="62" t="s">
+      <c r="F16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J16" s="92" t="s">
+      <c r="J16" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71" t="s">
+    <row r="17" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="33" t="s">
+      <c r="D17" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F17" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="62" t="s">
+      <c r="F17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J17" s="92" t="s">
+      <c r="J17" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="71" t="s">
+    <row r="18" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="62" t="s">
+      <c r="F18" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="J18" s="60" t="s">
+      <c r="J18" s="57" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71" t="s">
+    <row r="19" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="33" t="s">
+      <c r="D19" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F19" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="62" t="s">
+      <c r="F19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="J19" s="92" t="s">
+      <c r="J19" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71" t="s">
+    <row r="20" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>301</v>
-      </c>
-      <c r="H20" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="62" t="s">
+      <c r="D20" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>298</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="57" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71" t="s">
+    <row r="21" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="33" t="s">
+      <c r="D21" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J21" s="92" t="s">
+      <c r="F21" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="71" t="s">
+    <row r="22" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="68" t="s">
         <v>239</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="62">
+      <c r="F22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="59">
         <v>5200</v>
       </c>
-      <c r="J22" s="60" t="s">
+      <c r="J22" s="57" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="71" t="s">
+    <row r="23" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="68" t="s">
         <v>237</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="G23" s="72" t="s">
-        <v>269</v>
-      </c>
-      <c r="H23" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="62">
+      <c r="D23" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G23" s="69" t="s">
+        <v>266</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="59">
         <v>1</v>
       </c>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="57" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+    <row r="24" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A24" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D24" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F24" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="62" t="s">
+      <c r="F24" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="60" t="s">
+      <c r="J24" s="57" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="71" t="s">
+    <row r="25" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -5276,30 +5266,30 @@
       <c r="D25" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="G25" s="72" t="s">
-        <v>270</v>
-      </c>
-      <c r="H25" s="37" t="s">
+      <c r="E25" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G25" s="69" t="s">
+        <v>267</v>
+      </c>
+      <c r="H25" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J25" s="60" t="s">
+      <c r="J25" s="57" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -5308,158 +5298,158 @@
       <c r="D26" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="89" t="s">
-        <v>288</v>
-      </c>
-      <c r="F26" s="33" t="s">
+      <c r="E26" s="84" t="s">
+        <v>285</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G26" s="69" t="s">
         <v>268</v>
       </c>
-      <c r="G26" s="72" t="s">
-        <v>271</v>
-      </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J26" s="60" t="s">
+      <c r="J26" s="57" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="71" t="s">
+    <row r="27" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="68" t="s">
         <v>240</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="52" t="s">
+      <c r="C27" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="62" t="s">
+      <c r="F27" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="J27" s="60" t="s">
+      <c r="J27" s="57" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="71" t="s">
+    <row r="28" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H28" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="91">
+      <c r="D28" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="86">
         <v>44196</v>
       </c>
-      <c r="J28" s="60" t="s">
+      <c r="J28" s="57" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="71" t="s">
+    <row r="29" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H29" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I29" s="91">
+      <c r="D29" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="86">
         <v>43831</v>
       </c>
-      <c r="J29" s="60" t="s">
+      <c r="J29" s="57" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="G30" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="H30" s="37" t="s">
+      <c r="E30" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="G30" s="43" t="s">
+        <v>279</v>
+      </c>
+      <c r="H30" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J30" s="60" t="s">
+      <c r="J30" s="57" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="68" t="s">
         <v>236</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="47" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -5468,62 +5458,62 @@
       <c r="D31" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F31" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H31" s="37" t="s">
+      <c r="F31" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I31" s="18">
         <v>0</v>
       </c>
-      <c r="J31" s="60" t="s">
+      <c r="J31" s="57" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="83" t="s">
+      <c r="A32" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="G32" s="72" t="s">
-        <v>274</v>
-      </c>
-      <c r="H32" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="I32" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J32" s="60" t="s">
+      <c r="C32" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="57" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -5532,487 +5522,487 @@
       <c r="D33" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="86" t="s">
+      <c r="E33" s="81" t="s">
         <v>251</v>
       </c>
-      <c r="F33" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="88" t="s">
-        <v>38</v>
-      </c>
-      <c r="H33" s="37" t="s">
+      <c r="F33" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J33" s="61" t="s">
+      <c r="J33" s="58" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="71" t="s">
+    <row r="34" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A34" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H34" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" s="62" t="s">
+      <c r="F34" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J34" s="60" t="s">
+      <c r="J34" s="57" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+    <row r="35" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A35" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F35" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H35" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I35" s="62" t="s">
+      <c r="F35" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J35" s="60" t="s">
+      <c r="J35" s="57" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71" t="s">
+    <row r="36" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="68" t="s">
         <v>241</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="93">
+      <c r="C36" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="88">
         <v>44166</v>
       </c>
-      <c r="F36" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H36" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I36" s="65">
+      <c r="F36" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36" s="62">
         <v>43874</v>
       </c>
-      <c r="J36" s="60" t="s">
+      <c r="J36" s="57" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71" t="s">
+    <row r="37" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="33" t="s">
+      <c r="D37" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F37" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I37" s="65">
+      <c r="F37" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="62">
         <v>33187</v>
       </c>
-      <c r="J37" s="92" t="s">
+      <c r="J37" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="71" t="s">
+    <row r="38" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="33">
+      <c r="D38" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="31">
         <v>1</v>
       </c>
-      <c r="F38" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" s="73"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="92"/>
-    </row>
-    <row r="39" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="71" t="s">
+      <c r="F38" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H38" s="70"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="87"/>
+    </row>
+    <row r="39" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="33" t="s">
+      <c r="D39" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F39" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I39" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J39" s="60" t="s">
+      <c r="F39" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="57" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="71" t="s">
+    <row r="40" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="33" t="s">
+      <c r="D40" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F40" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="I40" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J40" s="60" t="s">
+      <c r="F40" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" s="57" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="48" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="71" t="s">
+    <row r="41" spans="1:10" s="46" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A41" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E41" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F41" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G41" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H41" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="62" t="s">
+      <c r="F41" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H41" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J41" s="60" t="s">
+      <c r="J41" s="57" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="71" t="s">
+    <row r="42" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="33" t="s">
+      <c r="D42" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F42" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H42" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I42" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J42" s="92" t="s">
+      <c r="F42" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G42" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I42" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J42" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="48" t="s">
-        <v>284</v>
-      </c>
-      <c r="B43" s="49" t="s">
+    <row r="43" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="B43" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="51" t="s">
+      <c r="D43" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="48" t="s">
-        <v>297</v>
-      </c>
-      <c r="G43" s="94"/>
-      <c r="H43" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I43" s="63" t="s">
-        <v>285</v>
-      </c>
-      <c r="J43" s="60" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="71" t="s">
+      <c r="E43" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="G43" s="89"/>
+      <c r="H43" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="J43" s="57" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="33" t="s">
+      <c r="D44" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F44" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G44" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I44" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="J44" s="60" t="s">
+      <c r="F44" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="57" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="71" t="s">
+    <row r="45" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="E45" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F45" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="62" t="s">
+      <c r="F45" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J45" s="92" t="s">
+      <c r="J45" s="87" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="71" t="s">
+    <row r="46" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="68" t="s">
         <v>243</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="50" t="s">
+      <c r="C46" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="52" t="s">
+      <c r="D46" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="62" t="s">
+      <c r="E46" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="J46" s="60" t="s">
+      <c r="J46" s="57" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="71" t="s">
+    <row r="47" spans="1:10" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="68" t="s">
         <v>244</v>
       </c>
-      <c r="B47" s="49" t="s">
+      <c r="B47" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="50" t="s">
+      <c r="C47" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="52" t="s">
+      <c r="D47" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="E47" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F47" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G47" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H47" s="73"/>
-      <c r="I47" s="62"/>
-      <c r="J47" s="60"/>
-    </row>
-    <row r="48" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="71" t="s">
+      <c r="F47" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="70"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="57"/>
+    </row>
+    <row r="48" spans="1:10" s="46" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A48" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="49" t="s">
+      <c r="C48" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="F48" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="G48" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="H48" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="I48" s="62" t="s">
+      <c r="D48" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="H48" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J48" s="60" t="s">
+      <c r="J48" s="57" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="70"/>
+      <c r="A90" s="67"/>
     </row>
   </sheetData>
   <phoneticPr fontId="25" type="noConversion"/>
@@ -6032,32 +6022,32 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="58"/>
-      <c r="B1" s="58"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>